<commit_message>
Avances, TP al punto 30 y CORRECCIŃ diagrama P14.A
</commit_message>
<xml_diff>
--- a/TP2/Punto14.A.xlsx
+++ b/TP2/Punto14.A.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
   <si>
     <t xml:space="preserve">Punto14.A</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">(R2, 1, 2) (R2, 5, 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7&lt;</t>
   </si>
   <si>
     <t xml:space="preserve">(R1, 2, 3) (R3, 4, 3)</t>
@@ -113,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +173,14 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -186,7 +197,14 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC9211E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -195,6 +213,14 @@
       <i val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -210,7 +236,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <bgColor rgb="FFC9211E"/>
       </patternFill>
     </fill>
     <fill>
@@ -221,7 +247,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF729FCF"/>
+        <fgColor rgb="FF5983B0"/>
         <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
@@ -301,12 +327,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -362,31 +388,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -398,7 +428,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -414,7 +444,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -422,75 +452,67 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -521,7 +543,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB4C7E7"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF729FCF"/>
+      <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -551,13 +573,13 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF5983B0"/>
       <rgbColor rgb="FF77BC65"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -743,15 +765,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL14"/>
+  <dimension ref="A1:AP14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q14" activeCellId="0" sqref="Q14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,6 +900,18 @@
       <c r="AL2" s="8" t="n">
         <v>30</v>
       </c>
+      <c r="AM2" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="AN2" s="8" t="n">
+        <v>32</v>
+      </c>
+      <c r="AO2" s="8" t="n">
+        <v>33</v>
+      </c>
+      <c r="AP2" s="8" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="n">
@@ -906,53 +940,55 @@
       <c r="J3" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="14" t="n">
+      <c r="K3" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="L3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="M3" s="15" t="s">
         <v>8</v>
       </c>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
       <c r="Q3" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="R3" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="R3" s="14" t="n">
+      <c r="S3" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="T3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="U3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="V3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="14" t="n">
+      <c r="W3" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="W3" s="14" t="n">
+      <c r="X3" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="Y3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="Z3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="Z3" s="16" t="s">
+      <c r="AA3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="AA3" s="13" t="s">
+      <c r="AB3" s="18"/>
+      <c r="AC3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AB3" s="17"/>
-      <c r="AC3" s="18"/>
       <c r="AD3" s="18"/>
       <c r="AE3" s="18"/>
       <c r="AF3" s="18"/>
@@ -962,6 +998,10 @@
       <c r="AJ3" s="18"/>
       <c r="AK3" s="18"/>
       <c r="AL3" s="18"/>
+      <c r="AM3" s="19"/>
+      <c r="AN3" s="19"/>
+      <c r="AO3" s="19"/>
+      <c r="AP3" s="19"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="n">
@@ -981,57 +1021,71 @@
       <c r="G4" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="H4" s="17"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="14" t="n">
-        <v>1</v>
-      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="16"/>
       <c r="L4" s="14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M4" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="N4" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="O4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="P4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="14" t="n">
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="20"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE4" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="Z4" s="16" t="s">
+      <c r="AF4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="20" t="s">
+      <c r="AG4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="AB4" s="17"/>
-      <c r="AC4" s="21" t="s">
+      <c r="AH4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="18"/>
-      <c r="AE4" s="18"/>
-      <c r="AF4" s="18"/>
-      <c r="AG4" s="18"/>
-      <c r="AH4" s="18"/>
       <c r="AI4" s="18"/>
       <c r="AJ4" s="18"/>
       <c r="AK4" s="18"/>
       <c r="AL4" s="18"/>
+      <c r="AM4" s="19"/>
+      <c r="AN4" s="19"/>
+      <c r="AO4" s="19"/>
+      <c r="AP4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="n">
@@ -1051,49 +1105,53 @@
       <c r="G5" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="17"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="8"/>
       <c r="J5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="19"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="17"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="18"/>
       <c r="AC5" s="18"/>
       <c r="AD5" s="18"/>
-      <c r="AE5" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="21" t="n">
-        <v>2</v>
-      </c>
-      <c r="AG5" s="21" t="n">
+      <c r="AE5" s="21"/>
+      <c r="AF5" s="21"/>
+      <c r="AG5" s="21"/>
+      <c r="AH5" s="18"/>
+      <c r="AI5" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK5" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="AH5" s="18"/>
-      <c r="AI5" s="18"/>
-      <c r="AJ5" s="21" t="n">
+      <c r="AL5" s="21"/>
+      <c r="AM5" s="19"/>
+      <c r="AN5" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="AK5" s="22" t="s">
+      <c r="AO5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="AL5" s="21" t="s">
+      <c r="AP5" s="22" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1115,63 +1173,66 @@
       <c r="G6" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
       <c r="K6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="V6" s="16" t="s">
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="W6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="W6" s="16" t="s">
+      <c r="X6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA6" s="14" t="n">
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE6" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="AB6" s="14" t="n">
+      <c r="AF6" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="AC6" s="18"/>
-      <c r="AD6" s="21" t="n">
+      <c r="AG6" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="AE6" s="22" t="s">
+      <c r="AH6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="AF6" s="22" t="s">
+      <c r="AI6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="AG6" s="22" t="s">
+      <c r="AJ6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="AH6" s="21" t="n">
+      <c r="AL6" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="AI6" s="21" t="n">
-        <v>7</v>
-      </c>
-      <c r="AJ6" s="18"/>
-      <c r="AK6" s="18"/>
-      <c r="AL6" s="18"/>
+      <c r="AM6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN6" s="19"/>
+      <c r="AO6" s="19"/>
+      <c r="AP6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="n">
@@ -1184,56 +1245,58 @@
         <v>5</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
       <c r="M7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="17"/>
+      <c r="N7" s="18"/>
       <c r="O7" s="13" t="n">
         <v>1</v>
       </c>
       <c r="P7" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="Q7" s="16" t="s">
+      <c r="Q7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="R7" s="16" t="s">
+      <c r="R7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="S7" s="14" t="n">
+      <c r="S7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="T7" s="4" t="n">
+      <c r="U7" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="U7" s="16" t="s">
+      <c r="V7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="V7" s="16" t="s">
+      <c r="W7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="W7" s="16" t="s">
+      <c r="X7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="X7" s="14" t="s">
+      <c r="Y7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
-      <c r="AA7" s="17"/>
-      <c r="AB7" s="17"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="18"/>
+      <c r="AB7" s="18"/>
       <c r="AC7" s="18"/>
       <c r="AD7" s="18"/>
       <c r="AE7" s="18"/>
@@ -1244,51 +1307,55 @@
       <c r="AJ7" s="18"/>
       <c r="AK7" s="18"/>
       <c r="AL7" s="18"/>
+      <c r="AM7" s="19"/>
+      <c r="AN7" s="19"/>
+      <c r="AO7" s="19"/>
+      <c r="AP7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="s">
-        <v>18</v>
+      <c r="A8" s="24" t="s">
+        <v>19</v>
       </c>
       <c r="B8" s="8"/>
-      <c r="C8" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="28"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="25"/>
-      <c r="X8" s="25"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="25"/>
-      <c r="AA8" s="25"/>
-      <c r="AB8" s="25"/>
+      <c r="C8" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="26"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="26"/>
+      <c r="W8" s="26"/>
+      <c r="X8" s="26"/>
+      <c r="Y8" s="27"/>
+      <c r="Z8" s="26"/>
+      <c r="AA8" s="26"/>
+      <c r="AB8" s="26"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="31"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33" t="s">
+      <c r="A9" s="30" t="s">
         <v>21</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="H9" s="34" t="n">
         <v>1</v>
@@ -1305,48 +1372,48 @@
       <c r="L9" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="M9" s="35" t="n">
+      <c r="M9" s="37" t="n">
         <v>5</v>
       </c>
-      <c r="N9" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="37"/>
-      <c r="V9" s="37"/>
-      <c r="W9" s="37"/>
-      <c r="X9" s="37"/>
-      <c r="Y9" s="38"/>
-      <c r="Z9" s="37"/>
-      <c r="AA9" s="37"/>
-      <c r="AB9" s="37"/>
-      <c r="AC9" s="39"/>
-      <c r="AD9" s="39"/>
-      <c r="AE9" s="39"/>
-      <c r="AF9" s="39"/>
-      <c r="AG9" s="39"/>
-      <c r="AH9" s="39"/>
-      <c r="AI9" s="39"/>
-      <c r="AJ9" s="39"/>
-      <c r="AK9" s="39"/>
-      <c r="AL9" s="39"/>
+      <c r="N9" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="41" t="n">
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="40" t="n">
         <v>2</v>
       </c>
       <c r="I10" s="35" t="n">
@@ -1355,7 +1422,7 @@
       <c r="J10" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="K10" s="42" t="n">
+      <c r="K10" s="41" t="n">
         <v>4</v>
       </c>
       <c r="L10" s="36" t="n">
@@ -1364,200 +1431,208 @@
       <c r="M10" s="35" t="n">
         <v>4</v>
       </c>
-      <c r="N10" s="35" t="n">
+      <c r="N10" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="O10" s="42" t="n">
         <v>4</v>
       </c>
-      <c r="O10" s="37"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="37"/>
-      <c r="S10" s="37"/>
-      <c r="T10" s="37"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="37"/>
-      <c r="W10" s="37"/>
-      <c r="X10" s="37"/>
-      <c r="Y10" s="37"/>
-      <c r="Z10" s="37"/>
-      <c r="AA10" s="37"/>
-      <c r="AB10" s="37"/>
-      <c r="AC10" s="39"/>
-      <c r="AD10" s="39"/>
-      <c r="AE10" s="39"/>
-      <c r="AF10" s="39"/>
-      <c r="AG10" s="39"/>
-      <c r="AH10" s="39"/>
-      <c r="AI10" s="39"/>
-      <c r="AJ10" s="39"/>
-      <c r="AK10" s="39"/>
-      <c r="AL10" s="39"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="9"/>
+      <c r="AL10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="32"/>
-      <c r="G11" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="41" t="n">
+      <c r="F11" s="33"/>
+      <c r="G11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="40" t="n">
         <v>3</v>
       </c>
       <c r="I11" s="43" t="n">
         <v>3</v>
       </c>
-      <c r="J11" s="44"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="44"/>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="44"/>
-      <c r="S11" s="44"/>
-      <c r="T11" s="44"/>
-      <c r="U11" s="44"/>
-      <c r="V11" s="44"/>
-      <c r="W11" s="44"/>
-      <c r="X11" s="44"/>
-      <c r="Y11" s="45"/>
-      <c r="Z11" s="44"/>
-      <c r="AA11" s="44"/>
-      <c r="AB11" s="44"/>
-      <c r="AC11" s="39"/>
-      <c r="AD11" s="39"/>
-      <c r="AE11" s="39"/>
-      <c r="AF11" s="39"/>
-      <c r="AG11" s="39"/>
-      <c r="AH11" s="39"/>
-      <c r="AI11" s="39"/>
-      <c r="AJ11" s="39"/>
-      <c r="AK11" s="39"/>
-      <c r="AL11" s="39"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="45"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="45"/>
+      <c r="U11" s="45"/>
+      <c r="V11" s="45"/>
+      <c r="W11" s="45"/>
+      <c r="X11" s="45"/>
+      <c r="Y11" s="44"/>
+      <c r="Z11" s="45"/>
+      <c r="AA11" s="45"/>
+      <c r="AB11" s="45"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="32"/>
-      <c r="G12" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="39"/>
-      <c r="S12" s="39"/>
-      <c r="T12" s="39"/>
-      <c r="U12" s="39"/>
-      <c r="V12" s="39"/>
-      <c r="W12" s="39"/>
-      <c r="X12" s="39"/>
-      <c r="Y12" s="39"/>
-      <c r="Z12" s="39"/>
-      <c r="AA12" s="39"/>
-      <c r="AB12" s="39"/>
-      <c r="AC12" s="39"/>
-      <c r="AD12" s="39"/>
-      <c r="AE12" s="39"/>
-      <c r="AF12" s="39"/>
-      <c r="AG12" s="39"/>
-      <c r="AH12" s="39"/>
-      <c r="AI12" s="39"/>
-      <c r="AJ12" s="39"/>
-      <c r="AK12" s="39"/>
-      <c r="AL12" s="39"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="35" t="n">
+        <v>5</v>
+      </c>
+      <c r="J12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+      <c r="AJ12" s="9"/>
+      <c r="AK12" s="9"/>
+      <c r="AL12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F13" s="32"/>
-      <c r="G13" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="47" t="n">
+      <c r="F13" s="33"/>
+      <c r="G13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="35" t="n">
         <v>4</v>
       </c>
-      <c r="J13" s="47" t="n">
+      <c r="J13" s="35" t="n">
         <v>4</v>
       </c>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="39"/>
-      <c r="S13" s="39"/>
-      <c r="T13" s="39"/>
-      <c r="U13" s="39"/>
-      <c r="V13" s="39"/>
-      <c r="W13" s="39"/>
-      <c r="X13" s="39"/>
-      <c r="Y13" s="39"/>
-      <c r="Z13" s="39"/>
-      <c r="AA13" s="39"/>
-      <c r="AB13" s="39"/>
-      <c r="AC13" s="39"/>
-      <c r="AD13" s="39"/>
-      <c r="AE13" s="39"/>
-      <c r="AF13" s="39"/>
-      <c r="AG13" s="39"/>
-      <c r="AH13" s="39"/>
-      <c r="AI13" s="39"/>
-      <c r="AJ13" s="39"/>
-      <c r="AK13" s="39"/>
-      <c r="AL13" s="39"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="9"/>
+      <c r="AI13" s="9"/>
+      <c r="AJ13" s="9"/>
+      <c r="AK13" s="9"/>
+      <c r="AL13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G14" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="47" t="n">
-        <v>2</v>
-      </c>
-      <c r="I14" s="47" t="n">
+      <c r="G14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="35" t="n">
         <v>5</v>
       </c>
-      <c r="J14" s="47" t="n">
-        <v>2</v>
-      </c>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="39"/>
-      <c r="Z14" s="18"/>
-      <c r="AA14" s="18"/>
-      <c r="AB14" s="18"/>
-      <c r="AC14" s="18"/>
-      <c r="AD14" s="18"/>
-      <c r="AE14" s="18"/>
-      <c r="AF14" s="18"/>
-      <c r="AG14" s="18"/>
-      <c r="AH14" s="18"/>
-      <c r="AI14" s="18"/>
-      <c r="AJ14" s="18"/>
-      <c r="AK14" s="18"/>
-      <c r="AL14" s="18"/>
+      <c r="J14" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="K14" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="8"/>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="8"/>
+      <c r="AG14" s="8"/>
+      <c r="AH14" s="8"/>
+      <c r="AI14" s="8"/>
+      <c r="AJ14" s="8"/>
+      <c r="AK14" s="8"/>
+      <c r="AL14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>